<commit_message>
Home page test cases added for actitime applications
</commit_message>
<xml_diff>
--- a/actitime/src/test/resource/com/acti/time/resource/altitimelogintestdata.xlsx
+++ b/actitime/src/test/resource/com/acti/time/resource/altitimelogintestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malli\Desktop\Automation Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC97DF0-37DB-471E-BD88-94EB70E9E107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD7495E-9E11-4F3E-9A7E-90014285DB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>P2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>mmanubrolu</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,6 +470,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>